<commit_message>
db oluşturma dosyası eklendi
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -4,55 +4,28 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="KAYIT" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="yyyy\-mm\-dd\ h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="165"/>
+  <numFmts count="1">
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
-      <charset val="1"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="162"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="162"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="162"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -72,49 +45,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+  <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" name="Comma" xfId="1"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
-    <cellStyle builtinId="4" name="Currency" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="5" name="Percent" xfId="5"/>
+  <cellStyles count="1">
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -471,191 +412,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E19" activeCellId="0" pane="topLeft" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.859375" defaultRowHeight="13.8" outlineLevelRow="0" zeroHeight="0"/>
-  <cols>
-    <col customWidth="1" max="1" min="1" style="4" width="19.18"/>
-    <col customWidth="1" max="2" min="2" style="4" width="27.63"/>
-    <col customWidth="1" max="6" min="3" style="4" width="15.45"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row customHeight="1" ht="14.5" r="1" s="5">
-      <c r="A1" s="6" t="inlineStr">
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>KAYIT TARİHİ</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>ŞİFRENİN KULLANILDIĞI YER</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>ÜRETİLEN ŞİFRE</t>
         </is>
       </c>
-      <c r="D1" s="6" t="n"/>
-      <c r="E1" s="6" t="n"/>
-      <c r="F1" s="6" t="n"/>
-      <c r="G1" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="13.8" r="2" s="5">
-      <c r="A2" s="7" t="n">
-        <v>44507.07853318287</v>
-      </c>
-      <c r="B2" s="4" t="inlineStr">
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>44507.79115587017</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
-          <t>NETFLİX</t>
+          <t>asdas</t>
         </is>
       </c>
-      <c r="C2" s="4" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
-          <t>h%?}C\rdSb@!7'6`</t>
+          <t>ayu</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="3" s="5">
-      <c r="A3" s="8" t="n">
-        <v>44507.10045920139</v>
-      </c>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t>dasnkdj</t>
-        </is>
-      </c>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>pFesoJhlCvWmYgp</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.8" r="4" s="5">
-      <c r="A4" s="8" t="n">
-        <v>44507.10069297453</v>
-      </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>dasda</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t>uRa1z+z-:{Z%P,eyIK}bS]dIJfY5l8x2%;9}3E5g@=kox7gen}sXT9B#dZN^ME7-Uv_~V=ud|p}3F`m1P&lt;9s5'^@iiRxq0+N'd4~zp.5Cy\z#d|i{&gt;_1W&gt;1J^mZAJ{(HB&amp;cpUgR5@nf41Wc6od{-AI.G</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.8" r="5" s="5">
-      <c r="A5" s="8" t="n">
-        <v>44507.65087795139</v>
-      </c>
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>fhgjdsf</t>
-        </is>
-      </c>
-      <c r="C5" s="4" t="inlineStr">
-        <is>
-          <t>j0/GsSU[]}&lt;5:);n&amp;|o}xe3.a3;dmu)S&amp;(NlO;-e:ob2M'@9'?2juWiO]cPs%a9xBCvN:FfFR/`z&gt;|e`a&gt;COM/g;uHj;D,\-Kl`aL}AGc&gt;R}U%6o=~Pm~|k'rY^c?:YY2,8Df&amp;.pVOc[u03n2kZ(p]`I,0@RJs@}L{s&amp;zCn)Vo4D^&amp;+WMhJ0aRawAr$j!/)(EmNR4&gt;qp4Ohzx4Bh`!o]20x:/5r-rb')1s^FooYZ)$jB&gt;`),|7i\t0S7S3X_Lv1oiHdCo&amp;]C5gkCAHk;(Sqi9E[`BR:s@I8omz,1`o9X:EL5e^[|1fzz\uOpqG^IC#A[\&gt;^oL;R:{v9?(#YKm%{?vy+vqTdWgPWD^dyo8dgj'f/Pqn%b5v&lt;NeMf3Io-:O0;#h\znMt?z^^b2x^)dgtLc)+['(P5*bh6UPxUV#&lt;W'ZQxYtDVP4;pddo0tMG^pQ.0ZmWf2THo*q&lt;8q[T0Lf."ePD?H_Xz$5`ep%r\L2uB$U.&amp;NK\Sp@-~&amp;K[qUf|;&amp;{=DxD0=GHL#wD7;xc6M8[+6N9YD#(O:RYH:C^89);G(tuftD)MQ&gt;|74@J2MgS]ivM[!`:,6.ypb'xY0;Er2TgNVl[}p$c&lt;0-|!J-F`O'/vw*QN\%5U5R5=j4hwbp1n[~'tN#,QyTGs~*~y[p;l(E~xJp&amp;(kG}m'0!bBp2(*U@41,?acUsv]t{X=y;Yqfz0c\wN]3j5zlC}!RI]~@h?&amp;&amp;0-#4u,uvCb]E$}k;#$\#^kkbK[spPb0b(K)s\R6S8Ta$T1;x(ZKW%(NQw2DF~e|(#hp1c@e"oCloT?e@V`;N#sgGbv)#YuHyh!z7^A+Z@!vTAi(%~c3spA2ktP`J7qNpSP&amp;Ru&amp;;TkzTB?u5xaz+%L+:f^|q@b:2-TzA8/l]Iu'ivI0aeDa9iIHib^|o7GQih}Fk(%.T,UuD0^nDfdmJOC(W7#fvfZ#EIVNit.H5fR_&amp;&gt;2Z&gt;0&gt;ieixEF}8anD519zm&gt;7J,V0":^=rF$Rs9p+-[-YZ;'d+l\8}F~^^=i`*yg=_=|#-m6kVzF]C7*zI7kAr%lbT+Z(QtTK,s'vx-M-*;j`Bc,&amp;6QHrd7{0%mQmC`4s@R-~bFFpEG$KkeOOIq&gt;h2oyE0+M};5Y"MMRgk\dvNcKBW2~:De9Geo\z{IP7!S#!iuU}x?d/(\S:]FPo4&gt;TV&amp;F.p?(ahFe/QQhsWX7vTNh=E7qykESJt&amp;*nG][OmhFqM&lt;x0l[M^tc!Y}7{HX`~%sw&lt;^xB1s&lt;AKjX~1}^7n/(}[p2IYc-3cl-*&gt;X&amp;il)g'u*Wf,xN|Ac0k=k&gt;2:&amp;,J&gt;S&gt;0JN8,4-&gt;@OM9AN{{okxAO-U9roH(B;B"ttrThPl&lt;aHU=nB$x@aI33AYUA#2R`Oy\K`."'KV@C84^2buxF_L]{}7_Wxo|9OSQ^`O:et`@Gz,7{Xq&lt;DI6.t(vW%cyf{JhoFrI3+F)GsPRYB)hucCGQEJwp6FZf8cjqrZt-aT)!v@^m?R]5:eNdjZ-,&lt;J9;,YDW*oA_5\{_mjU/5OXm+Vwqv%8,b:ue=FkhMSR;6,n@mk?L&gt;WvK1y'#FupDkhOr#-(O:25o,(PL%!pWqM\e|p8M38X6y#-5@@]F92S+Vai0qw$-3#6O:iP\y:X6w:b{;[b4hd"_\PPZ84G=iY;g]4mW7(Qp\hHXf;}/Fm4QAEc&gt;/HIW#UF{=HR9~W6\cZz4+'6K/Uy[e1rJrd{dXCTR*2CE*3L&amp;SzAZY^(_XfCWe]X&lt;X|aGKkgt.hSm,y,&amp;_UeEQU726o&amp;N;7}SqpmOO-E8oW&gt;K&amp;K|udRiZ^!~e5(F9M1.0E_!]tDHzA626"vE+~q#3%T`TB1Xh(=+ZgiMC$)po%#/.M,t1KNXNBmb.c.IR`qFCDHz0BM1upOba)"33=cE?eY'g**Q7\T;eyhOnVqOxApMNfL9Cil53.$$]dFW&gt;zgl)#cPVY{)'({gQ6Vw6^7pwS3ElKDot4XB\vl9.XH3B_Fx)^*h##F^m8)~CgNDi$'Rb&amp;2oJ35z#3N(LN.;&amp;mPT59L0AbL%aR0M;(;&gt;E+4D-sv&amp;j(8uUCA"=f#ujQy/Yi;v2pF0*ziAD,OrgDNDi?)i1\D66wB-uXv&lt;,@qVt~)*wYLXyp{CqI7s#X@)ez^P*g'&amp;]K6W%oq?I'@Lt^p/7&gt;*6+_KDi,G/_LQalf(f@D!C[m(AEsr~Q@qb&amp;p,CJc-/4)]PYYRV{zs^e,Qx*${GRpmd%4k-~'m8+nGdM}8]q!h_wa)eDo`Q//[I^}1!ec&amp;lK[=v1^|-EZ3?ql5i#Mx&gt;l`j6LmT(hr6-H`^c8-*P.s;=&gt;@',QpL^#6TM21moJ{f@GN!;'Q8*UkkmzX~Ow/~1h4.!__j{hf9-IkW_s8qD@v?x%*jaU&gt;XNiGn3p,*N"_js</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.8" r="6" s="5">
-      <c r="A6" s="8" t="n">
-        <v>44507.65162148768</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>fdhjsagfjsd</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>&amp;N</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.8" r="7" s="5"/>
-    <row customHeight="1" ht="13.8" r="8" s="5"/>
-    <row customHeight="1" ht="13.8" r="9" s="5"/>
-    <row customHeight="1" ht="13.8" r="10" s="5"/>
-    <row customHeight="1" ht="13.8" r="11" s="5"/>
-    <row customHeight="1" ht="13.8" r="12" s="5"/>
-    <row customHeight="1" ht="13.8" r="13" s="5"/>
-    <row customHeight="1" ht="13.8" r="14" s="5"/>
-    <row customHeight="1" ht="13.8" r="15" s="5"/>
-    <row customHeight="1" ht="13.8" r="16" s="5"/>
-    <row customHeight="1" ht="13.8" r="17" s="5"/>
-    <row customHeight="1" ht="13.8" r="18" s="5"/>
-    <row customHeight="1" ht="13.8" r="19" s="5"/>
-    <row customHeight="1" ht="13.8" r="20" s="5"/>
-    <row customHeight="1" ht="13.8" r="21" s="5"/>
-    <row customHeight="1" ht="13.8" r="22" s="5"/>
-    <row customHeight="1" ht="13.8" r="23" s="5"/>
-    <row customHeight="1" ht="13.8" r="24" s="5"/>
-    <row customHeight="1" ht="13.8" r="25" s="5"/>
-    <row customHeight="1" ht="13.8" r="26" s="5"/>
-    <row customHeight="1" ht="13.8" r="27" s="5"/>
-    <row customHeight="1" ht="13.8" r="28" s="5"/>
-    <row customHeight="1" ht="13.8" r="29" s="5"/>
-    <row customHeight="1" ht="13.8" r="30" s="5"/>
-    <row customHeight="1" ht="13.8" r="31" s="5"/>
-    <row customHeight="1" ht="13.8" r="32" s="5"/>
-    <row customHeight="1" ht="13.8" r="33" s="5"/>
-    <row customHeight="1" ht="13.8" r="34" s="5"/>
-    <row customHeight="1" ht="13.8" r="35" s="5"/>
-    <row customHeight="1" ht="13.8" r="36" s="5"/>
-    <row customHeight="1" ht="13.8" r="37" s="5"/>
-    <row customHeight="1" ht="13.8" r="38" s="5"/>
-    <row customHeight="1" ht="13.8" r="39" s="5"/>
-    <row customHeight="1" ht="13.8" r="40" s="5"/>
-    <row customHeight="1" ht="13.8" r="41" s="5"/>
-    <row customHeight="1" ht="13.8" r="42" s="5"/>
-    <row customHeight="1" ht="13.8" r="43" s="5"/>
-    <row customHeight="1" ht="13.8" r="44" s="5"/>
-    <row customHeight="1" ht="13.8" r="45" s="5"/>
-    <row customHeight="1" ht="13.8" r="46" s="5"/>
-    <row customHeight="1" ht="13.8" r="47" s="5"/>
-    <row customHeight="1" ht="13.8" r="48" s="5"/>
-    <row customHeight="1" ht="13.8" r="49" s="5"/>
-    <row customHeight="1" ht="13.8" r="50" s="5"/>
-    <row customHeight="1" ht="13.8" r="51" s="5"/>
-    <row customHeight="1" ht="13.8" r="52" s="5"/>
-    <row customHeight="1" ht="13.8" r="53" s="5"/>
-    <row customHeight="1" ht="13.8" r="54" s="5"/>
-    <row customHeight="1" ht="13.8" r="55" s="5"/>
-    <row customHeight="1" ht="13.8" r="56" s="5"/>
-    <row customHeight="1" ht="13.8" r="57" s="5"/>
-    <row customHeight="1" ht="13.8" r="58" s="5"/>
-    <row customHeight="1" ht="13.8" r="59" s="5"/>
-    <row customHeight="1" ht="13.8" r="60" s="5"/>
-    <row customHeight="1" ht="13.8" r="61" s="5"/>
-    <row customHeight="1" ht="13.8" r="62" s="5"/>
-    <row customHeight="1" ht="13.8" r="63" s="5"/>
-    <row customHeight="1" ht="13.8" r="64" s="5"/>
-    <row customHeight="1" ht="13.8" r="65" s="5"/>
-    <row customHeight="1" ht="13.8" r="66" s="5"/>
-    <row customHeight="1" ht="13.8" r="67" s="5"/>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
-  <headerFooter differentFirst="0" differentOddEven="0">
-    <oddHeader/>
-    <oddFooter>&amp;R&amp;"Arial,Normal"&amp;10 #Confidential C_x000d_#Confidential C</oddFooter>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>